<commit_message>
first version of the interface + production code
</commit_message>
<xml_diff>
--- a/knn_result.xlsx
+++ b/knn_result.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General Informations" sheetId="3" r:id="rId1"/>
@@ -658,7 +658,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -802,11 +802,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -872,6 +898,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1292,8 +1324,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="E2:J105"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:J26"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="L34" sqref="L34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1615,10 +1647,10 @@
       </c>
     </row>
     <row r="29" spans="5:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="E29" s="19" t="s">
+      <c r="E29" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="F29" s="19"/>
+      <c r="F29" s="24"/>
       <c r="H29" s="5" t="s">
         <v>5</v>
       </c>
@@ -1924,10 +1956,10 @@
       </c>
     </row>
     <row r="55" spans="5:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="E55" s="19" t="s">
+      <c r="E55" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="F55" s="19"/>
+      <c r="F55" s="24"/>
       <c r="H55" s="5" t="s">
         <v>5</v>
       </c>
@@ -2233,10 +2265,10 @@
       </c>
     </row>
     <row r="81" spans="5:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="E81" s="19" t="s">
+      <c r="E81" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="F81" s="19"/>
+      <c r="F81" s="24"/>
       <c r="H81" s="5" t="s">
         <v>5</v>
       </c>
@@ -2557,8 +2589,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78B84295-B517-4CF6-95F4-93D327A7FB03}">
   <dimension ref="E2:J104"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q83" sqref="Q83"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E102" sqref="E102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>